<commit_message>
almost final for DOM
</commit_message>
<xml_diff>
--- a/DOM_Banner/output/dept_banner/Abd Assalam Qannus_2023.xlsx
+++ b/DOM_Banner/output/dept_banner/Abd Assalam Qannus_2023.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AH2"/>
+  <dimension ref="A1:P2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -360,354 +360,164 @@
     <row r="1" s="1" customFormat="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
+          <t>authors_name</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
           <t>id</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="C1" s="1" t="inlineStr">
         <is>
           <t>display_name</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>author</t>
-        </is>
-      </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>ab</t>
+          <t>publication_date</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>publication_date</t>
+          <t>so</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>so</t>
+          <t>host_organization</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>so_id</t>
+          <t>url</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>host_organization</t>
+          <t>license</t>
         </is>
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
-          <t>issn_l</t>
+          <t>version</t>
         </is>
       </c>
       <c r="J1" s="1" t="inlineStr">
         <is>
-          <t>url</t>
+          <t>oa_status</t>
         </is>
       </c>
       <c r="K1" s="1" t="inlineStr">
         <is>
-          <t>pdf_url</t>
+          <t>language</t>
         </is>
       </c>
       <c r="L1" s="1" t="inlineStr">
         <is>
-          <t>license</t>
+          <t>cited_by_count</t>
         </is>
       </c>
       <c r="M1" s="1" t="inlineStr">
         <is>
-          <t>version</t>
+          <t>publication_year</t>
         </is>
       </c>
       <c r="N1" s="1" t="inlineStr">
         <is>
-          <t>first_page</t>
+          <t>pmid</t>
         </is>
       </c>
       <c r="O1" s="1" t="inlineStr">
         <is>
-          <t>last_page</t>
+          <t>doi</t>
         </is>
       </c>
       <c r="P1" s="1" t="inlineStr">
         <is>
-          <t>volume</t>
-        </is>
-      </c>
-      <c r="Q1" s="1" t="inlineStr">
-        <is>
-          <t>issue</t>
-        </is>
-      </c>
-      <c r="R1" s="1" t="inlineStr">
-        <is>
-          <t>is_oa</t>
-        </is>
-      </c>
-      <c r="S1" s="1" t="inlineStr">
-        <is>
-          <t>is_oa_anywhere</t>
-        </is>
-      </c>
-      <c r="T1" s="1" t="inlineStr">
-        <is>
-          <t>oa_status</t>
-        </is>
-      </c>
-      <c r="U1" s="1" t="inlineStr">
-        <is>
-          <t>oa_url</t>
-        </is>
-      </c>
-      <c r="V1" s="1" t="inlineStr">
-        <is>
-          <t>any_repository_has_fulltext</t>
-        </is>
-      </c>
-      <c r="W1" s="1" t="inlineStr">
-        <is>
-          <t>language</t>
-        </is>
-      </c>
-      <c r="X1" s="1" t="inlineStr">
-        <is>
-          <t>grants</t>
-        </is>
-      </c>
-      <c r="Y1" s="1" t="inlineStr">
-        <is>
-          <t>cited_by_count</t>
-        </is>
-      </c>
-      <c r="Z1" s="1" t="inlineStr">
-        <is>
-          <t>publication_year</t>
-        </is>
-      </c>
-      <c r="AA1" s="1" t="inlineStr">
-        <is>
-          <t>cited_by_api_url</t>
-        </is>
-      </c>
-      <c r="AB1" s="1" t="inlineStr">
-        <is>
-          <t>ids</t>
-        </is>
-      </c>
-      <c r="AC1" s="1" t="inlineStr">
-        <is>
-          <t>doi</t>
-        </is>
-      </c>
-      <c r="AD1" s="1" t="inlineStr">
-        <is>
           <t>type</t>
-        </is>
-      </c>
-      <c r="AE1" s="1" t="inlineStr">
-        <is>
-          <t>referenced_works</t>
-        </is>
-      </c>
-      <c r="AF1" s="1" t="inlineStr">
-        <is>
-          <t>related_works</t>
-        </is>
-      </c>
-      <c r="AG1" s="1" t="inlineStr">
-        <is>
-          <t>is_paratext</t>
-        </is>
-      </c>
-      <c r="AH1" s="1" t="inlineStr">
-        <is>
-          <t>is_retracted</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
+          <t>Srilekha Sridhara, Ahmet B. Gungor, Halil Erol, Mohanad Al-Obaidi, Tirdad T. Zangeneh, Edward J. Bedrick, Venkatesh Kumar Ariyamuthu, Aneesha Shetty, Abd Assalam Qannus, Katherine Mendoza, Sangeetha Murugapandian, Gaurav Gupta, Bekir Tanrıöver</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
           <t>https://openalex.org/W4367309455</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr">
+      <c r="C2" t="inlineStr">
         <is>
           <t>Lack of effectiveness of Bebtelovimab monoclonal antibody among high-risk patients with SARS-Cov-2 Omicron during BA.2, BA.2.12.1 and BA.5 subvariants dominated era</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>list(au_id = c("https://openalex.org/A5044512783", "https://openalex.org/A5011527972", "https://openalex.org/A5020624718", "https://openalex.org/A5045990380", "https://openalex.org/A5076993071", "https://openalex.org/A5014060810", "https://openalex.org/A5022492748", "https://openalex.org/A5017534571", "https://openalex.org/A5059968219", "https://openalex.org/A5016503578", "https://openalex.org/A5070439382", "https://openalex.org/A5044372095", "https://openalex.org/A5016874418"), au_display_name = c("Srilekha Sridhara", 
-"Ahmet B. Gungor", "Halil Erol", "Mohanad Al-Obaidi", "Tirdad T. Zangeneh", "Edward J. Bedrick", "Venkatesh Kumar Ariyamuthu", "Aneesha Shetty", "Abd Assalam Qannus", "Katherine Mendoza", "Sangeetha Murugapandian", "Gaurav Gupta", "Bekir Tanrıöver"), au_orcid = c(NA, NA, "https://orcid.org/0000-0001-5760-4276", "https://orcid.org/0000-0002-5189-6594", "https://orcid.org/0000-0002-9035-2952", NA, NA, NA, NA, "https://orcid.org/0000-0001-9618-2336", "https://orcid.org/0000-0002-9145-5283", "https://orcid.org/0000-0001-7941-0229", 
-"https://orcid.org/0000-0002-2378-9302"), author_position = c("first", "middle", "middle", "middle", "middle", "middle", "middle", "middle", "middle", "middle", "middle", "middle", "last"), au_affiliation_raw = c("Division of Nephrology, College of Medicine, The University of Arizona, Tucson, Arizona, United States of America", "Division of Nephrology, The Banner University Medical Center, Tucson, Arizona, United States of America", "Division of Nephrology, College of Medicine, The University of Arizona, Tucson, Arizona, United States of America", 
-"Division of Infectious Diseases, College of Medicine, The University of Arizona, Tucson, Arizona, United States of America", "Division of Infectious Diseases, College of Medicine, The University of Arizona, Tucson, Arizona, United States of America", "Department of Epidemiology and Biostatistics, College of Public Health, The University of Arizona, Tucson, Arizona, United States of America", "Division of Nephrology, College of Medicine, The University of Arizona, Tucson, Arizona, United States of America", 
-"Division of Nephrology, College of Medicine, The University of Arizona, Tucson, Arizona, United States of America", "Division of Nephrology, College of Medicine, The University of Arizona, Tucson, Arizona, United States of America", "Division of Nephrology, College of Medicine, The University of Arizona, Tucson, Arizona, United States of America", "Division of Nephrology, College of Medicine, The University of Arizona, Tucson, Arizona, United States of America", "Division of Nephrology, Virginia Commonwealth University, Richmond, Virginia, United States of America", 
-"Division of Nephrology, College of Medicine, The University of Arizona, Tucson, Arizona, United States of America"), institution_id = c("https://openalex.org/I138006243", "https://openalex.org/I4210124665", "https://openalex.org/I138006243", "https://openalex.org/I138006243", "https://openalex.org/I138006243", "https://openalex.org/I138006243", "https://openalex.org/I138006243", "https://openalex.org/I138006243", "https://openalex.org/I138006243", "https://openalex.org/I138006243", "https://openalex.org/I138006243", 
-"https://openalex.org/I184840846", "https://openalex.org/I138006243"), institution_display_name = c("University of Arizona", "Banner - University Medical Center Tucson", "University of Arizona", "University of Arizona", "University of Arizona", "University of Arizona", "University of Arizona", "University of Arizona", "University of Arizona", "University of Arizona", "University of Arizona", "Virginia Commonwealth University", "University of Arizona"), institution_ror = c("https://ror.org/03m2x1q45", 
-"https://ror.org/02xbk5j62", "https://ror.org/03m2x1q45", "https://ror.org/03m2x1q45", "https://ror.org/03m2x1q45", "https://ror.org/03m2x1q45", "https://ror.org/03m2x1q45", "https://ror.org/03m2x1q45", "https://ror.org/03m2x1q45", "https://ror.org/03m2x1q45", "https://ror.org/03m2x1q45", "https://ror.org/02nkdxk79", "https://ror.org/03m2x1q45"), institution_country_code = c("US", "US", "US", "US", "US", "US", "US", "US", "US", "US", "US", "US", "US"), institution_type = c("education", "healthcare", 
-"education", "education", "education", "education", "education", "education", "education", "education", "education", "education", "education"), institution_lineage = c("https://openalex.org/I138006243, https://openalex.org/I3132585960", "https://openalex.org/I4210124665", "https://openalex.org/I138006243, https://openalex.org/I3132585960", "https://openalex.org/I138006243, https://openalex.org/I3132585960", "https://openalex.org/I138006243, https://openalex.org/I3132585960", "https://openalex.org/I138006243, https://openalex.org/I3132585960", 
-"https://openalex.org/I138006243, https://openalex.org/I3132585960", "https://openalex.org/I138006243, https://openalex.org/I3132585960", "https://openalex.org/I138006243, https://openalex.org/I3132585960", "https://openalex.org/I138006243, https://openalex.org/I3132585960", "https://openalex.org/I138006243, https://openalex.org/I3132585960", "https://openalex.org/I184840846", "https://openalex.org/I138006243, https://openalex.org/I3132585960"))</t>
-        </is>
-      </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Severe acute respiratory syndrome coronavirus 2 (SARS-CoV-2) Omicron subvariants are expected to be resistant to Bebtelovimab (BEB) monoclonal antibody (MAb) and the real-world experience regarding its effectiveness is scarce. This retrospective cohort study reports a data analysis in Banner Healthcare System (a large not-for-profit organization) between 4/5/2022 and 8/1/2022 and included 19,778 Coronavirus disease-19 (COVID-19) positive (by PCR or direct antigen testing) patients who were selected from Cerner-Electronic Health Record after the exclusions criteria were met. The study index date for cohort was determined as the date of BEB MAb administration or the date of the first positive COVID-19 testing. The cohort consist of COVID-19 infected patients who received BEB MAb (N = 1,091) compared to propensity score (PS) matched control (N = 1,091). The primary composite outcome was the incidence of 30-day all-cause hospitalization and/or mortality. All statistical analyses were conducted on the paired (matched) dataset. For the primary composite outcome, the event counts and percentages were reported. Ninety-five percent Clopper-Pearson confidence intervals for percentages were computed. The study cohorts were 1:1 propensity matched without replacement across 26 covariates using an optimal matching algorithm that minimizes the sum of absolute pairwise distance across the matched sample after fitting and using logistic regression as the distance function. The pairs were matched exactly on patient vaccination status, BMI group, age group and diabetes status. Compared to the PS matched control group (2.6%; 95% confidence interval [CI]: 1.7%, 3.7%), BEB MAb use (2.2%; 95% CI: 1.4%, 3.3%) did not significantly reduce the incidence of the primary outcome (p = 0.67). In the subgroup analysis, we observed similar no-difference trends regarding the primary outcomes for the propensity rematched BEB MAb treated and untreated groups, stratified by patient vaccination status, age (&lt;65 years or ≥65), and immunocompromised status (patients with HIV/AIDS or solid organ transplants or malignancy including lymphoproliferative disorder). The number needed to treat (1/0.026-0.022) with BEB MAb was 250 to avoid one hospitalization and/or death over 30 days. The BEB MAb use lacked efficacy in patients with SARS-CoV-2 Omicron subvariants (mainly BA.2, BA.2.12.1, and BA.5) in the Banner Healthcare System in the Southwestern United States.</t>
+          <t>2023-04-28</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>2023-04-28</t>
+          <t>PLOS ONE</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>PLOS ONE</t>
+          <t>Public Library of Science</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>https://openalex.org/S202381698</t>
+          <t>https://doi.org/10.1371/journal.pone.0279326</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>Public Library of Science</t>
+          <t>cc-by</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>1932-6203</t>
+          <t>publishedVersion</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
         <is>
+          <t>gold</t>
+        </is>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>en</t>
+        </is>
+      </c>
+      <c r="L2" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="M2" t="inlineStr">
+        <is>
+          <t>2023</t>
+        </is>
+      </c>
+      <c r="N2" t="inlineStr">
+        <is>
+          <t>https://pubmed.ncbi.nlm.nih.gov/37115780</t>
+        </is>
+      </c>
+      <c r="O2" t="inlineStr">
+        <is>
           <t>https://doi.org/10.1371/journal.pone.0279326</t>
         </is>
       </c>
-      <c r="K2" t="inlineStr">
-        <is>
-          <t>https://journals.plos.org/plosone/article/file?id=10.1371/journal.pone.0279326&amp;type=printable</t>
-        </is>
-      </c>
-      <c r="L2" t="inlineStr">
-        <is>
-          <t>cc-by</t>
-        </is>
-      </c>
-      <c r="M2" t="inlineStr">
-        <is>
-          <t>publishedVersion</t>
-        </is>
-      </c>
-      <c r="N2" t="inlineStr">
-        <is>
-          <t>e0279326</t>
-        </is>
-      </c>
-      <c r="O2" t="inlineStr">
-        <is>
-          <t>e0279326</t>
-        </is>
-      </c>
       <c r="P2" t="inlineStr">
         <is>
-          <t>18</t>
-        </is>
-      </c>
-      <c r="Q2" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
-      <c r="R2" t="inlineStr">
-        <is>
-          <t>TRUE</t>
-        </is>
-      </c>
-      <c r="S2" t="inlineStr">
-        <is>
-          <t>TRUE</t>
-        </is>
-      </c>
-      <c r="T2" t="inlineStr">
-        <is>
-          <t>gold</t>
-        </is>
-      </c>
-      <c r="U2" t="inlineStr">
-        <is>
-          <t>https://journals.plos.org/plosone/article/file?id=10.1371/journal.pone.0279326&amp;type=printable</t>
-        </is>
-      </c>
-      <c r="V2" t="inlineStr">
-        <is>
-          <t>TRUE</t>
-        </is>
-      </c>
-      <c r="W2" t="inlineStr">
-        <is>
-          <t>en</t>
-        </is>
-      </c>
-      <c r="X2" t="inlineStr">
-        <is>
-          <t>c(funder = "https://openalex.org/F4320330230", funder_display_name = "AiCuris")</t>
-        </is>
-      </c>
-      <c r="Y2" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
-      <c r="Z2" t="inlineStr">
-        <is>
-          <t>2023</t>
-        </is>
-      </c>
-      <c r="AA2" t="inlineStr">
-        <is>
-          <t>https://api.openalex.org/works?filter=cites:W4367309455</t>
-        </is>
-      </c>
-      <c r="AB2" t="inlineStr">
-        <is>
-          <t>c(openalex = "https://openalex.org/W4367309455", doi = "https://doi.org/10.1371/journal.pone.0279326", pmid = "https://pubmed.ncbi.nlm.nih.gov/37115780")</t>
-        </is>
-      </c>
-      <c r="AC2" t="inlineStr">
-        <is>
-          <t>https://doi.org/10.1371/journal.pone.0279326</t>
-        </is>
-      </c>
-      <c r="AD2" t="inlineStr">
-        <is>
           <t>article</t>
-        </is>
-      </c>
-      <c r="AE2" t="inlineStr">
-        <is>
-          <t>c("https://openalex.org/W2036193982", "https://openalex.org/W2122771444", "https://openalex.org/W3008028633", "https://openalex.org/W3034312608", "https://openalex.org/W3090928025", "https://openalex.org/W4220729480", "https://openalex.org/W4220774106", "https://openalex.org/W4220886953", "https://openalex.org/W4220970752", "https://openalex.org/W4225263923", "https://openalex.org/W4225647476", "https://openalex.org/W4226342921", "https://openalex.org/W4282835288", "https://openalex.org/W4283026725", 
-"https://openalex.org/W4285727819", "https://openalex.org/W4286009139", "https://openalex.org/W4295899573", "https://openalex.org/W4296702018", "https://openalex.org/W4298086777", "https://openalex.org/W4298394671", "https://openalex.org/W4304117179", "https://openalex.org/W4310576518", "https://openalex.org/W4312019047")</t>
-        </is>
-      </c>
-      <c r="AF2" t="inlineStr">
-        <is>
-          <t>c("https://openalex.org/W2793335702", "https://openalex.org/W4210646467", "https://openalex.org/W2154948599", "https://openalex.org/W2913113213", "https://openalex.org/W4254083861", "https://openalex.org/W2090763189", "https://openalex.org/W2792027122", "https://openalex.org/W2792916732", "https://openalex.org/W3114266572", "https://openalex.org/W4240976644")</t>
-        </is>
-      </c>
-      <c r="AG2" t="inlineStr">
-        <is>
-          <t>FALSE</t>
-        </is>
-      </c>
-      <c r="AH2" t="inlineStr">
-        <is>
-          <t>FALSE</t>
         </is>
       </c>
     </row>

</xml_diff>